<commit_message>
Update levantamento BD CDVs via 1 e 2 (2).xlsx
</commit_message>
<xml_diff>
--- a/levantamento BD CDVs via 1 e 2 (2).xlsx
+++ b/levantamento BD CDVs via 1 e 2 (2).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e6a03ffa708fbd6b/Desktop/PI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muril\Documents\Sitcon\Sitcon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="647" documentId="11_9EFEF2A5D2E6054B5FFE7680DEDDA2C0995CD8D0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA0DE9E7-A6FB-454B-A1D3-00F8EE5B92A8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2268D48-0FD1-4885-8B2B-73E03DFAFF6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14385" yWindow="0" windowWidth="14520" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Equipamentos" sheetId="1" r:id="rId1"/>
@@ -1422,7 +1422,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1458,12 +1458,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="14">
@@ -1633,7 +1639,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1646,13 +1652,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1933,13 +1945,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:N139"/>
+  <dimension ref="B1:N137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L133" sqref="L133"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B103" sqref="B103:B113"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" customWidth="1"/>
@@ -1949,72 +1961,72 @@
     <col min="10" max="14" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="15" customHeight="1">
-      <c r="B1" s="12" t="s">
+    <row r="1" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="14"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="21"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="14"/>
-    </row>
-    <row r="2" spans="2:14" ht="15" customHeight="1">
-      <c r="B2" s="15" t="s">
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="16"/>
+    </row>
+    <row r="2" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="17"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="J2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="17"/>
-    </row>
-    <row r="3" spans="2:14" ht="15" customHeight="1">
-      <c r="B3" s="15"/>
-      <c r="C3" s="16" t="s">
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="13"/>
+    </row>
+    <row r="3" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="17"/>
+      <c r="C3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="16" t="s">
+      <c r="D3" s="12"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="17"/>
+      <c r="G3" s="13"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="16" t="s">
+      <c r="I3" s="17"/>
+      <c r="J3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="16"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="16" t="s">
+      <c r="K3" s="12"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="17"/>
-    </row>
-    <row r="4" spans="2:14" ht="15.75">
+      <c r="N3" s="13"/>
+    </row>
+    <row r="4" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="18"/>
       <c r="C4" s="2" t="s">
         <v>6</v>
@@ -2049,7 +2061,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="2:14" ht="15">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>15</v>
       </c>
@@ -2088,7 +2100,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="2:14" ht="15">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
@@ -2127,7 +2139,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="2:14" ht="15">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>26</v>
       </c>
@@ -2166,7 +2178,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="2:14" ht="15">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>37</v>
       </c>
@@ -2205,7 +2217,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="2:14" ht="15">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>31</v>
       </c>
@@ -2244,7 +2256,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="2:14" ht="15">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>55</v>
       </c>
@@ -2271,7 +2283,7 @@
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
     </row>
-    <row r="11" spans="2:14" ht="18.75">
+    <row r="11" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
         <v>59</v>
       </c>
@@ -2291,16 +2303,16 @@
         <v>58</v>
       </c>
       <c r="H11" s="1"/>
-      <c r="I11" s="12" t="s">
+      <c r="I11" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="14"/>
-    </row>
-    <row r="12" spans="2:14" ht="15.75">
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="16"/>
+    </row>
+    <row r="12" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>62</v>
       </c>
@@ -2320,18 +2332,18 @@
         <v>64</v>
       </c>
       <c r="H12" s="1"/>
-      <c r="I12" s="15" t="s">
+      <c r="I12" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="J12" s="16" t="s">
+      <c r="J12" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="K12" s="16"/>
-      <c r="L12" s="16"/>
-      <c r="M12" s="16"/>
-      <c r="N12" s="17"/>
-    </row>
-    <row r="13" spans="2:14" ht="15" customHeight="1">
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="13"/>
+    </row>
+    <row r="13" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>65</v>
       </c>
@@ -2351,18 +2363,18 @@
         <v>67</v>
       </c>
       <c r="H13" s="1"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="16" t="s">
+      <c r="I13" s="17"/>
+      <c r="J13" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="K13" s="16"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="16" t="s">
+      <c r="K13" s="12"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N13" s="17"/>
-    </row>
-    <row r="14" spans="2:14" ht="15.75">
+      <c r="N13" s="13"/>
+    </row>
+    <row r="14" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>40</v>
       </c>
@@ -2399,7 +2411,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="2:14" ht="15">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>49</v>
       </c>
@@ -2438,7 +2450,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="2:14" ht="15">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -2465,15 +2477,15 @@
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="2:14" ht="18.75">
-      <c r="B17" s="12" t="s">
+    <row r="17" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B17" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="14"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="16"/>
       <c r="H17" s="1"/>
       <c r="I17" s="5" t="s">
         <v>49</v>
@@ -2494,17 +2506,17 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="2:14" ht="15.75">
-      <c r="B18" s="15" t="s">
+    <row r="18" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="17"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="13"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -2513,28 +2525,28 @@
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
     </row>
-    <row r="19" spans="2:14" ht="15" customHeight="1">
-      <c r="B19" s="15"/>
-      <c r="C19" s="16" t="s">
+    <row r="19" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="17"/>
+      <c r="C19" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="16"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="16" t="s">
+      <c r="D19" s="12"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G19" s="17"/>
+      <c r="G19" s="13"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="12" t="s">
+      <c r="I19" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="14"/>
-    </row>
-    <row r="20" spans="2:14" ht="15" customHeight="1">
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="16"/>
+    </row>
+    <row r="20" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="18"/>
       <c r="C20" s="2" t="s">
         <v>92</v>
@@ -2552,18 +2564,18 @@
         <v>95</v>
       </c>
       <c r="H20" s="1"/>
-      <c r="I20" s="15" t="s">
+      <c r="I20" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="J20" s="16" t="s">
+      <c r="J20" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="K20" s="16"/>
-      <c r="L20" s="16"/>
-      <c r="M20" s="16"/>
-      <c r="N20" s="17"/>
-    </row>
-    <row r="21" spans="2:14" ht="15" customHeight="1">
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="13"/>
+    </row>
+    <row r="21" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
         <v>26</v>
       </c>
@@ -2583,18 +2595,18 @@
         <v>98</v>
       </c>
       <c r="H21" s="1"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="16" t="s">
+      <c r="I21" s="17"/>
+      <c r="J21" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="K21" s="16"/>
-      <c r="L21" s="17"/>
-      <c r="M21" s="16" t="s">
+      <c r="K21" s="12"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N21" s="17"/>
-    </row>
-    <row r="22" spans="2:14" ht="15.75">
+      <c r="N21" s="13"/>
+    </row>
+    <row r="22" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>31</v>
       </c>
@@ -2631,7 +2643,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="2:14" ht="15">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>40</v>
       </c>
@@ -2670,7 +2682,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="24" spans="2:14" ht="15">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>49</v>
       </c>
@@ -2709,7 +2721,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="2:14" ht="15">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -2736,7 +2748,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="26" spans="2:14" ht="15">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -2763,7 +2775,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="27" spans="2:14" ht="15">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -2778,72 +2790,72 @@
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
     </row>
-    <row r="28" spans="2:14" ht="15" customHeight="1">
-      <c r="B28" s="12" t="s">
+    <row r="28" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="14"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="16"/>
       <c r="H28" s="1"/>
-      <c r="I28" s="12" t="s">
+      <c r="I28" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-      <c r="N28" s="14"/>
-    </row>
-    <row r="29" spans="2:14" ht="15" customHeight="1">
-      <c r="B29" s="15" t="s">
+      <c r="J28" s="20"/>
+      <c r="K28" s="20"/>
+      <c r="L28" s="20"/>
+      <c r="M28" s="20"/>
+      <c r="N28" s="21"/>
+    </row>
+    <row r="29" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C29" s="16" t="s">
+      <c r="C29" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="17"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="13"/>
       <c r="H29" s="1"/>
-      <c r="I29" s="15" t="s">
+      <c r="I29" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="J29" s="16" t="s">
+      <c r="J29" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="K29" s="16"/>
-      <c r="L29" s="16"/>
-      <c r="M29" s="16"/>
-      <c r="N29" s="17"/>
-    </row>
-    <row r="30" spans="2:14" ht="15" customHeight="1">
-      <c r="B30" s="15"/>
-      <c r="C30" s="16" t="s">
+      <c r="K29" s="12"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="13"/>
+    </row>
+    <row r="30" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="17"/>
+      <c r="C30" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D30" s="16"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="16" t="s">
+      <c r="D30" s="12"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G30" s="17"/>
+      <c r="G30" s="13"/>
       <c r="H30" s="1"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="16" t="s">
+      <c r="I30" s="17"/>
+      <c r="J30" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="K30" s="16"/>
-      <c r="L30" s="17"/>
-      <c r="M30" s="16" t="s">
+      <c r="K30" s="12"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N30" s="17"/>
-    </row>
-    <row r="31" spans="2:14" ht="15.75">
+      <c r="N30" s="13"/>
+    </row>
+    <row r="31" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="18"/>
       <c r="C31" s="2" t="s">
         <v>131</v>
@@ -2878,7 +2890,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="32" spans="2:14" ht="15">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B32" s="10" t="s">
         <v>119</v>
       </c>
@@ -2917,7 +2929,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="2:14" ht="15">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>62</v>
       </c>
@@ -2956,7 +2968,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="34" spans="2:14" ht="15">
+    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>40</v>
       </c>
@@ -2995,7 +3007,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="2:14" ht="15">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>49</v>
       </c>
@@ -3034,7 +3046,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="2:14" ht="15">
+    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -3061,15 +3073,15 @@
         <v>157</v>
       </c>
     </row>
-    <row r="37" spans="2:14" ht="18.75">
-      <c r="B37" s="12" t="s">
+    <row r="37" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B37" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="14"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="16"/>
       <c r="H37" s="1"/>
       <c r="I37" s="5" t="s">
         <v>55</v>
@@ -3090,17 +3102,17 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="2:14" ht="15.75">
-      <c r="B38" s="15" t="s">
+    <row r="38" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B38" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C38" s="16" t="s">
+      <c r="C38" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D38" s="16"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="17"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="13"/>
       <c r="H38" s="1"/>
       <c r="I38" s="5" t="s">
         <v>59</v>
@@ -3121,17 +3133,17 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="2:14" ht="15" customHeight="1">
-      <c r="B39" s="15"/>
-      <c r="C39" s="16" t="s">
+    <row r="39" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="17"/>
+      <c r="C39" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D39" s="16"/>
-      <c r="E39" s="17"/>
-      <c r="F39" s="16" t="s">
+      <c r="D39" s="12"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G39" s="17"/>
+      <c r="G39" s="13"/>
       <c r="H39" s="1"/>
       <c r="I39" s="5" t="s">
         <v>62</v>
@@ -3152,7 +3164,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="2:14" ht="15.75">
+    <row r="40" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B40" s="18"/>
       <c r="C40" s="2" t="s">
         <v>161</v>
@@ -3170,26 +3182,26 @@
         <v>164</v>
       </c>
       <c r="H40" s="1"/>
-      <c r="I40" s="5" t="s">
+      <c r="I40" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="J40" s="6" t="s">
+      <c r="J40" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="K40" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="L40" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="M40" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="N40" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="41" spans="2:14" ht="15">
+      <c r="K40" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="L40" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="M40" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="N40" s="24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
         <v>22</v>
       </c>
@@ -3228,7 +3240,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="42" spans="2:14" ht="15">
+    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="s">
         <v>26</v>
       </c>
@@ -3267,7 +3279,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="43" spans="2:14" ht="15">
+    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
         <v>31</v>
       </c>
@@ -3294,7 +3306,7 @@
       <c r="M43" s="1"/>
       <c r="N43" s="1"/>
     </row>
-    <row r="44" spans="2:14" ht="18.75">
+    <row r="44" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B44" s="5" t="s">
         <v>40</v>
       </c>
@@ -3314,16 +3326,16 @@
         <v>183</v>
       </c>
       <c r="H44" s="1"/>
-      <c r="I44" s="12" t="s">
+      <c r="I44" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="J44" s="13"/>
-      <c r="K44" s="13"/>
-      <c r="L44" s="13"/>
-      <c r="M44" s="13"/>
-      <c r="N44" s="14"/>
-    </row>
-    <row r="45" spans="2:14" ht="15.75">
+      <c r="J44" s="15"/>
+      <c r="K44" s="15"/>
+      <c r="L44" s="15"/>
+      <c r="M44" s="15"/>
+      <c r="N44" s="16"/>
+    </row>
+    <row r="45" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
         <v>49</v>
       </c>
@@ -3343,18 +3355,18 @@
         <v>189</v>
       </c>
       <c r="H45" s="1"/>
-      <c r="I45" s="15" t="s">
+      <c r="I45" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="J45" s="16" t="s">
+      <c r="J45" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="K45" s="16"/>
-      <c r="L45" s="16"/>
-      <c r="M45" s="16"/>
-      <c r="N45" s="17"/>
-    </row>
-    <row r="46" spans="2:14" ht="15" customHeight="1">
+      <c r="K45" s="12"/>
+      <c r="L45" s="12"/>
+      <c r="M45" s="12"/>
+      <c r="N45" s="13"/>
+    </row>
+    <row r="46" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -3362,26 +3374,26 @@
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
-      <c r="I46" s="15"/>
-      <c r="J46" s="16" t="s">
+      <c r="I46" s="17"/>
+      <c r="J46" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="K46" s="16"/>
-      <c r="L46" s="17"/>
-      <c r="M46" s="16" t="s">
+      <c r="K46" s="12"/>
+      <c r="L46" s="13"/>
+      <c r="M46" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N46" s="17"/>
-    </row>
-    <row r="47" spans="2:14" ht="18.75">
-      <c r="B47" s="12" t="s">
+      <c r="N46" s="13"/>
+    </row>
+    <row r="47" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B47" s="14" t="s">
         <v>190</v>
       </c>
-      <c r="C47" s="13"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="14"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="16"/>
       <c r="H47" s="1"/>
       <c r="I47" s="18"/>
       <c r="J47" s="2" t="s">
@@ -3400,17 +3412,17 @@
         <v>194</v>
       </c>
     </row>
-    <row r="48" spans="2:14" ht="15.75">
-      <c r="B48" s="15" t="s">
+    <row r="48" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B48" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C48" s="16" t="s">
+      <c r="C48" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D48" s="16"/>
-      <c r="E48" s="16"/>
-      <c r="F48" s="16"/>
-      <c r="G48" s="17"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="13"/>
       <c r="H48" s="1"/>
       <c r="I48" s="5" t="s">
         <v>26</v>
@@ -3431,17 +3443,17 @@
         <v>196</v>
       </c>
     </row>
-    <row r="49" spans="2:14" ht="15" customHeight="1">
-      <c r="B49" s="15"/>
-      <c r="C49" s="16" t="s">
+    <row r="49" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="17"/>
+      <c r="C49" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D49" s="16"/>
-      <c r="E49" s="17"/>
-      <c r="F49" s="16" t="s">
+      <c r="D49" s="12"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G49" s="17"/>
+      <c r="G49" s="13"/>
       <c r="H49" s="1"/>
       <c r="I49" s="5" t="s">
         <v>37</v>
@@ -3462,7 +3474,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="50" spans="2:14" ht="15.75">
+    <row r="50" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B50" s="18"/>
       <c r="C50" s="2" t="s">
         <v>198</v>
@@ -3499,7 +3511,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="51" spans="2:14" ht="15">
+    <row r="51" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B51" s="10" t="s">
         <v>37</v>
       </c>
@@ -3538,7 +3550,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="52" spans="2:14" ht="15">
+    <row r="52" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="s">
         <v>31</v>
       </c>
@@ -3577,7 +3589,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="53" spans="2:14" ht="15">
+    <row r="53" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B53" s="5" t="s">
         <v>40</v>
       </c>
@@ -3604,7 +3616,7 @@
       <c r="M53" s="1"/>
       <c r="N53" s="1"/>
     </row>
-    <row r="54" spans="2:14" ht="18.75">
+    <row r="54" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B54" s="5" t="s">
         <v>49</v>
       </c>
@@ -3624,16 +3636,16 @@
         <v>225</v>
       </c>
       <c r="H54" s="1"/>
-      <c r="I54" s="12" t="s">
+      <c r="I54" s="14" t="s">
         <v>226</v>
       </c>
-      <c r="J54" s="13"/>
-      <c r="K54" s="13"/>
-      <c r="L54" s="13"/>
-      <c r="M54" s="13"/>
-      <c r="N54" s="14"/>
-    </row>
-    <row r="55" spans="2:14" ht="15.75">
+      <c r="J54" s="15"/>
+      <c r="K54" s="15"/>
+      <c r="L54" s="15"/>
+      <c r="M54" s="15"/>
+      <c r="N54" s="16"/>
+    </row>
+    <row r="55" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -3641,49 +3653,49 @@
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
-      <c r="I55" s="15" t="s">
+      <c r="I55" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="J55" s="16" t="s">
+      <c r="J55" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="K55" s="16"/>
-      <c r="L55" s="16"/>
-      <c r="M55" s="16"/>
-      <c r="N55" s="17"/>
-    </row>
-    <row r="56" spans="2:14" ht="15" customHeight="1">
-      <c r="B56" s="12" t="s">
+      <c r="K55" s="12"/>
+      <c r="L55" s="12"/>
+      <c r="M55" s="12"/>
+      <c r="N55" s="13"/>
+    </row>
+    <row r="56" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="14" t="s">
         <v>227</v>
       </c>
-      <c r="C56" s="13"/>
-      <c r="D56" s="13"/>
-      <c r="E56" s="13"/>
-      <c r="F56" s="13"/>
-      <c r="G56" s="14"/>
+      <c r="C56" s="15"/>
+      <c r="D56" s="15"/>
+      <c r="E56" s="15"/>
+      <c r="F56" s="15"/>
+      <c r="G56" s="16"/>
       <c r="H56" s="1"/>
-      <c r="I56" s="15"/>
-      <c r="J56" s="16" t="s">
+      <c r="I56" s="17"/>
+      <c r="J56" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="K56" s="16"/>
-      <c r="L56" s="17"/>
-      <c r="M56" s="16" t="s">
+      <c r="K56" s="12"/>
+      <c r="L56" s="13"/>
+      <c r="M56" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N56" s="17"/>
-    </row>
-    <row r="57" spans="2:14" ht="15.75">
-      <c r="B57" s="15" t="s">
+      <c r="N56" s="13"/>
+    </row>
+    <row r="57" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B57" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C57" s="16" t="s">
+      <c r="C57" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D57" s="16"/>
-      <c r="E57" s="16"/>
-      <c r="F57" s="16"/>
-      <c r="G57" s="17"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="12"/>
+      <c r="F57" s="12"/>
+      <c r="G57" s="13"/>
       <c r="H57" s="1"/>
       <c r="I57" s="18"/>
       <c r="J57" s="2" t="s">
@@ -3702,17 +3714,17 @@
         <v>231</v>
       </c>
     </row>
-    <row r="58" spans="2:14" ht="15" customHeight="1">
-      <c r="B58" s="15"/>
-      <c r="C58" s="16" t="s">
+    <row r="58" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="17"/>
+      <c r="C58" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D58" s="16"/>
-      <c r="E58" s="17"/>
-      <c r="F58" s="16" t="s">
+      <c r="D58" s="12"/>
+      <c r="E58" s="13"/>
+      <c r="F58" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G58" s="17"/>
+      <c r="G58" s="13"/>
       <c r="H58" s="1"/>
       <c r="I58" s="10" t="s">
         <v>55</v>
@@ -3733,7 +3745,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="59" spans="2:14" ht="15.75">
+    <row r="59" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B59" s="18"/>
       <c r="C59" s="2" t="s">
         <v>235</v>
@@ -3770,7 +3782,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="2:14" ht="15">
+    <row r="60" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B60" s="10" t="s">
         <v>55</v>
       </c>
@@ -3809,7 +3821,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="61" spans="2:14" ht="15">
+    <row r="61" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B61" s="5" t="s">
         <v>40</v>
       </c>
@@ -3848,7 +3860,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="62" spans="2:14" ht="15">
+    <row r="62" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B62" s="5" t="s">
         <v>49</v>
       </c>
@@ -3875,7 +3887,7 @@
       <c r="M62" s="1"/>
       <c r="N62" s="1"/>
     </row>
-    <row r="63" spans="2:14" ht="15">
+    <row r="63" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
@@ -3890,72 +3902,72 @@
       <c r="M63" s="1"/>
       <c r="N63" s="1"/>
     </row>
-    <row r="64" spans="2:14" ht="15" customHeight="1">
-      <c r="B64" s="12" t="s">
+    <row r="64" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="14" t="s">
         <v>258</v>
       </c>
-      <c r="C64" s="13"/>
-      <c r="D64" s="13"/>
-      <c r="E64" s="13"/>
-      <c r="F64" s="13"/>
-      <c r="G64" s="14"/>
+      <c r="C64" s="15"/>
+      <c r="D64" s="15"/>
+      <c r="E64" s="15"/>
+      <c r="F64" s="15"/>
+      <c r="G64" s="16"/>
       <c r="H64" s="1"/>
-      <c r="I64" s="12" t="s">
+      <c r="I64" s="14" t="s">
         <v>259</v>
       </c>
-      <c r="J64" s="13"/>
-      <c r="K64" s="13"/>
-      <c r="L64" s="13"/>
-      <c r="M64" s="13"/>
-      <c r="N64" s="14"/>
-    </row>
-    <row r="65" spans="2:14" ht="15" customHeight="1">
-      <c r="B65" s="15" t="s">
+      <c r="J64" s="15"/>
+      <c r="K64" s="15"/>
+      <c r="L64" s="15"/>
+      <c r="M64" s="15"/>
+      <c r="N64" s="16"/>
+    </row>
+    <row r="65" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C65" s="16" t="s">
+      <c r="C65" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D65" s="16"/>
-      <c r="E65" s="16"/>
-      <c r="F65" s="16"/>
-      <c r="G65" s="17"/>
+      <c r="D65" s="12"/>
+      <c r="E65" s="12"/>
+      <c r="F65" s="12"/>
+      <c r="G65" s="13"/>
       <c r="H65" s="1"/>
-      <c r="I65" s="15" t="s">
+      <c r="I65" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="J65" s="16" t="s">
+      <c r="J65" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="K65" s="16"/>
-      <c r="L65" s="16"/>
-      <c r="M65" s="16"/>
-      <c r="N65" s="17"/>
-    </row>
-    <row r="66" spans="2:14" ht="15" customHeight="1">
-      <c r="B66" s="15"/>
-      <c r="C66" s="16" t="s">
+      <c r="K65" s="12"/>
+      <c r="L65" s="12"/>
+      <c r="M65" s="12"/>
+      <c r="N65" s="13"/>
+    </row>
+    <row r="66" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="17"/>
+      <c r="C66" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D66" s="16"/>
-      <c r="E66" s="17"/>
-      <c r="F66" s="16" t="s">
+      <c r="D66" s="12"/>
+      <c r="E66" s="13"/>
+      <c r="F66" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G66" s="17"/>
+      <c r="G66" s="13"/>
       <c r="H66" s="1"/>
-      <c r="I66" s="15"/>
-      <c r="J66" s="16" t="s">
+      <c r="I66" s="17"/>
+      <c r="J66" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="K66" s="16"/>
-      <c r="L66" s="17"/>
-      <c r="M66" s="16" t="s">
+      <c r="K66" s="12"/>
+      <c r="L66" s="13"/>
+      <c r="M66" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N66" s="17"/>
-    </row>
-    <row r="67" spans="2:14" ht="15.75">
+      <c r="N66" s="13"/>
+    </row>
+    <row r="67" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B67" s="18"/>
       <c r="C67" s="2" t="s">
         <v>260</v>
@@ -3990,7 +4002,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="68" spans="2:14" ht="15">
+    <row r="68" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B68" s="10" t="s">
         <v>119</v>
       </c>
@@ -4029,7 +4041,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="69" spans="2:14" ht="15">
+    <row r="69" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B69" s="5" t="s">
         <v>62</v>
       </c>
@@ -4068,7 +4080,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="70" spans="2:14" ht="15">
+    <row r="70" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B70" s="5" t="s">
         <v>40</v>
       </c>
@@ -4107,7 +4119,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="71" spans="2:14" ht="15">
+    <row r="71" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B71" s="5" t="s">
         <v>49</v>
       </c>
@@ -4146,7 +4158,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="72" spans="2:14" ht="15">
+    <row r="72" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
@@ -4161,72 +4173,72 @@
       <c r="M72" s="1"/>
       <c r="N72" s="1"/>
     </row>
-    <row r="73" spans="2:14" ht="15" customHeight="1">
-      <c r="B73" s="12" t="s">
+    <row r="73" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="14" t="s">
         <v>289</v>
       </c>
-      <c r="C73" s="13"/>
-      <c r="D73" s="13"/>
-      <c r="E73" s="13"/>
-      <c r="F73" s="13"/>
-      <c r="G73" s="14"/>
+      <c r="C73" s="15"/>
+      <c r="D73" s="15"/>
+      <c r="E73" s="15"/>
+      <c r="F73" s="15"/>
+      <c r="G73" s="16"/>
       <c r="H73" s="1"/>
-      <c r="I73" s="12" t="s">
+      <c r="I73" s="14" t="s">
         <v>290</v>
       </c>
-      <c r="J73" s="13"/>
-      <c r="K73" s="13"/>
-      <c r="L73" s="13"/>
-      <c r="M73" s="13"/>
-      <c r="N73" s="14"/>
-    </row>
-    <row r="74" spans="2:14" ht="15" customHeight="1">
-      <c r="B74" s="15" t="s">
+      <c r="J73" s="15"/>
+      <c r="K73" s="15"/>
+      <c r="L73" s="15"/>
+      <c r="M73" s="15"/>
+      <c r="N73" s="16"/>
+    </row>
+    <row r="74" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C74" s="16" t="s">
+      <c r="C74" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D74" s="16"/>
-      <c r="E74" s="16"/>
-      <c r="F74" s="16"/>
-      <c r="G74" s="17"/>
+      <c r="D74" s="12"/>
+      <c r="E74" s="12"/>
+      <c r="F74" s="12"/>
+      <c r="G74" s="13"/>
       <c r="H74" s="1"/>
-      <c r="I74" s="15" t="s">
+      <c r="I74" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="J74" s="16" t="s">
+      <c r="J74" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="K74" s="16"/>
-      <c r="L74" s="16"/>
-      <c r="M74" s="16"/>
-      <c r="N74" s="17"/>
-    </row>
-    <row r="75" spans="2:14" ht="15" customHeight="1">
-      <c r="B75" s="15"/>
-      <c r="C75" s="16" t="s">
+      <c r="K74" s="12"/>
+      <c r="L74" s="12"/>
+      <c r="M74" s="12"/>
+      <c r="N74" s="13"/>
+    </row>
+    <row r="75" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B75" s="17"/>
+      <c r="C75" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D75" s="16"/>
-      <c r="E75" s="17"/>
-      <c r="F75" s="16" t="s">
+      <c r="D75" s="12"/>
+      <c r="E75" s="13"/>
+      <c r="F75" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G75" s="17"/>
+      <c r="G75" s="13"/>
       <c r="H75" s="1"/>
-      <c r="I75" s="15"/>
-      <c r="J75" s="16" t="s">
+      <c r="I75" s="17"/>
+      <c r="J75" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="K75" s="16"/>
-      <c r="L75" s="17"/>
-      <c r="M75" s="16" t="s">
+      <c r="K75" s="12"/>
+      <c r="L75" s="13"/>
+      <c r="M75" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N75" s="17"/>
-    </row>
-    <row r="76" spans="2:14" ht="15.75">
+      <c r="N75" s="13"/>
+    </row>
+    <row r="76" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B76" s="18"/>
       <c r="C76" s="2" t="s">
         <v>291</v>
@@ -4261,7 +4273,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="77" spans="2:14" ht="15">
+    <row r="77" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B77" s="10" t="s">
         <v>299</v>
       </c>
@@ -4300,7 +4312,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="78" spans="2:14" ht="15">
+    <row r="78" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B78" s="5" t="s">
         <v>300</v>
       </c>
@@ -4339,7 +4351,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="79" spans="2:14" ht="15">
+    <row r="79" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B79" s="5" t="s">
         <v>40</v>
       </c>
@@ -4378,7 +4390,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="80" spans="2:14" ht="15">
+    <row r="80" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B80" s="5" t="s">
         <v>49</v>
       </c>
@@ -4417,7 +4429,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="81" spans="2:14" ht="15">
+    <row r="81" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
@@ -4444,7 +4456,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="82" spans="2:14" ht="15">
+    <row r="82" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
@@ -4459,72 +4471,72 @@
       <c r="M82" s="1"/>
       <c r="N82" s="1"/>
     </row>
-    <row r="83" spans="2:14" ht="15" customHeight="1">
-      <c r="B83" s="12" t="s">
+    <row r="83" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B83" s="14" t="s">
         <v>327</v>
       </c>
-      <c r="C83" s="13"/>
-      <c r="D83" s="13"/>
-      <c r="E83" s="13"/>
-      <c r="F83" s="13"/>
-      <c r="G83" s="14"/>
+      <c r="C83" s="15"/>
+      <c r="D83" s="15"/>
+      <c r="E83" s="15"/>
+      <c r="F83" s="15"/>
+      <c r="G83" s="16"/>
       <c r="H83" s="1"/>
-      <c r="I83" s="12" t="s">
+      <c r="I83" s="14" t="s">
         <v>328</v>
       </c>
-      <c r="J83" s="13"/>
-      <c r="K83" s="13"/>
-      <c r="L83" s="13"/>
-      <c r="M83" s="13"/>
-      <c r="N83" s="14"/>
-    </row>
-    <row r="84" spans="2:14" ht="15" customHeight="1">
-      <c r="B84" s="15" t="s">
+      <c r="J83" s="15"/>
+      <c r="K83" s="15"/>
+      <c r="L83" s="15"/>
+      <c r="M83" s="15"/>
+      <c r="N83" s="16"/>
+    </row>
+    <row r="84" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B84" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C84" s="16" t="s">
+      <c r="C84" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D84" s="16"/>
-      <c r="E84" s="16"/>
-      <c r="F84" s="16"/>
-      <c r="G84" s="17"/>
+      <c r="D84" s="12"/>
+      <c r="E84" s="12"/>
+      <c r="F84" s="12"/>
+      <c r="G84" s="13"/>
       <c r="H84" s="1"/>
-      <c r="I84" s="15" t="s">
+      <c r="I84" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="J84" s="16" t="s">
+      <c r="J84" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="K84" s="16"/>
-      <c r="L84" s="16"/>
-      <c r="M84" s="16"/>
-      <c r="N84" s="17"/>
-    </row>
-    <row r="85" spans="2:14" ht="15" customHeight="1">
-      <c r="B85" s="15"/>
-      <c r="C85" s="16" t="s">
+      <c r="K84" s="12"/>
+      <c r="L84" s="12"/>
+      <c r="M84" s="12"/>
+      <c r="N84" s="13"/>
+    </row>
+    <row r="85" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B85" s="17"/>
+      <c r="C85" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D85" s="16"/>
-      <c r="E85" s="17"/>
-      <c r="F85" s="16" t="s">
+      <c r="D85" s="12"/>
+      <c r="E85" s="13"/>
+      <c r="F85" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G85" s="17"/>
+      <c r="G85" s="13"/>
       <c r="H85" s="1"/>
-      <c r="I85" s="15"/>
-      <c r="J85" s="16" t="s">
+      <c r="I85" s="17"/>
+      <c r="J85" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="K85" s="16"/>
-      <c r="L85" s="17"/>
-      <c r="M85" s="16" t="s">
+      <c r="K85" s="12"/>
+      <c r="L85" s="13"/>
+      <c r="M85" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N85" s="17"/>
-    </row>
-    <row r="86" spans="2:14" ht="15.75">
+      <c r="N85" s="13"/>
+    </row>
+    <row r="86" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B86" s="18"/>
       <c r="C86" s="2" t="s">
         <v>329</v>
@@ -4559,7 +4571,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="87" spans="2:14" ht="15">
+    <row r="87" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B87" s="5" t="s">
         <v>300</v>
       </c>
@@ -4598,7 +4610,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="88" spans="2:14" ht="15">
+    <row r="88" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B88" s="5" t="s">
         <v>305</v>
       </c>
@@ -4637,7 +4649,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="89" spans="2:14" ht="15">
+    <row r="89" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B89" s="5" t="s">
         <v>310</v>
       </c>
@@ -4676,7 +4688,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="90" spans="2:14" ht="15">
+    <row r="90" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B90" s="5" t="s">
         <v>346</v>
       </c>
@@ -4715,7 +4727,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="91" spans="2:14" ht="15">
+    <row r="91" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B91" s="5" t="s">
         <v>40</v>
       </c>
@@ -4754,7 +4766,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="92" spans="2:14" ht="15">
+    <row r="92" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B92" s="5" t="s">
         <v>49</v>
       </c>
@@ -4793,7 +4805,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="93" spans="2:14" ht="15">
+    <row r="93" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
@@ -4820,7 +4832,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="94" spans="2:14" ht="15">
+    <row r="94" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
@@ -4847,7 +4859,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="95" spans="2:14" ht="15">
+    <row r="95" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
@@ -4874,7 +4886,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="96" spans="2:14" ht="15">
+    <row r="96" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
@@ -4901,7 +4913,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="97" spans="2:14" ht="15">
+    <row r="97" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
@@ -4916,72 +4928,72 @@
       <c r="M97" s="1"/>
       <c r="N97" s="1"/>
     </row>
-    <row r="98" spans="2:14" ht="15" customHeight="1">
-      <c r="B98" s="12" t="s">
+    <row r="98" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B98" s="14" t="s">
         <v>364</v>
       </c>
-      <c r="C98" s="13"/>
-      <c r="D98" s="13"/>
-      <c r="E98" s="13"/>
-      <c r="F98" s="13"/>
-      <c r="G98" s="14"/>
+      <c r="C98" s="15"/>
+      <c r="D98" s="15"/>
+      <c r="E98" s="15"/>
+      <c r="F98" s="15"/>
+      <c r="G98" s="16"/>
       <c r="H98" s="1"/>
-      <c r="I98" s="12" t="s">
+      <c r="I98" s="14" t="s">
         <v>365</v>
       </c>
-      <c r="J98" s="13"/>
-      <c r="K98" s="13"/>
-      <c r="L98" s="13"/>
-      <c r="M98" s="13"/>
-      <c r="N98" s="14"/>
-    </row>
-    <row r="99" spans="2:14" ht="15" customHeight="1">
-      <c r="B99" s="15" t="s">
+      <c r="J98" s="15"/>
+      <c r="K98" s="15"/>
+      <c r="L98" s="15"/>
+      <c r="M98" s="15"/>
+      <c r="N98" s="16"/>
+    </row>
+    <row r="99" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B99" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C99" s="16" t="s">
+      <c r="C99" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D99" s="16"/>
-      <c r="E99" s="16"/>
-      <c r="F99" s="16"/>
-      <c r="G99" s="17"/>
+      <c r="D99" s="12"/>
+      <c r="E99" s="12"/>
+      <c r="F99" s="12"/>
+      <c r="G99" s="13"/>
       <c r="H99" s="1"/>
-      <c r="I99" s="15" t="s">
+      <c r="I99" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="J99" s="16" t="s">
+      <c r="J99" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="K99" s="16"/>
-      <c r="L99" s="16"/>
-      <c r="M99" s="16"/>
-      <c r="N99" s="17"/>
-    </row>
-    <row r="100" spans="2:14" ht="15" customHeight="1">
-      <c r="B100" s="15"/>
-      <c r="C100" s="16" t="s">
+      <c r="K99" s="12"/>
+      <c r="L99" s="12"/>
+      <c r="M99" s="12"/>
+      <c r="N99" s="13"/>
+    </row>
+    <row r="100" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B100" s="17"/>
+      <c r="C100" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D100" s="16"/>
-      <c r="E100" s="17"/>
-      <c r="F100" s="16" t="s">
+      <c r="D100" s="12"/>
+      <c r="E100" s="13"/>
+      <c r="F100" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G100" s="17"/>
+      <c r="G100" s="13"/>
       <c r="H100" s="1"/>
-      <c r="I100" s="15"/>
-      <c r="J100" s="16" t="s">
+      <c r="I100" s="17"/>
+      <c r="J100" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="K100" s="16"/>
-      <c r="L100" s="17"/>
-      <c r="M100" s="16" t="s">
+      <c r="K100" s="12"/>
+      <c r="L100" s="13"/>
+      <c r="M100" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N100" s="17"/>
-    </row>
-    <row r="101" spans="2:14" ht="15.75">
+      <c r="N100" s="13"/>
+    </row>
+    <row r="101" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B101" s="18"/>
       <c r="C101" s="2" t="s">
         <v>366</v>
@@ -5016,7 +5028,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="102" spans="2:14" ht="15">
+    <row r="102" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B102" s="5" t="s">
         <v>299</v>
       </c>
@@ -5055,7 +5067,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="103" spans="2:14" ht="15">
+    <row r="103" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B103" s="5" t="s">
         <v>299</v>
       </c>
@@ -5094,7 +5106,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="104" spans="2:14" ht="15">
+    <row r="104" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B104" s="5" t="s">
         <v>270</v>
       </c>
@@ -5133,7 +5145,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="105" spans="2:14" ht="15">
+    <row r="105" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B105" s="5" t="s">
         <v>345</v>
       </c>
@@ -5172,7 +5184,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="106" spans="2:14" ht="15">
+    <row r="106" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B106" s="5" t="s">
         <v>300</v>
       </c>
@@ -5199,7 +5211,7 @@
       <c r="M106" s="1"/>
       <c r="N106" s="1"/>
     </row>
-    <row r="107" spans="2:14" ht="18.75">
+    <row r="107" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B107" s="5" t="s">
         <v>305</v>
       </c>
@@ -5219,16 +5231,16 @@
         <v>375</v>
       </c>
       <c r="H107" s="1"/>
-      <c r="I107" s="12" t="s">
+      <c r="I107" s="14" t="s">
         <v>388</v>
       </c>
-      <c r="J107" s="13"/>
-      <c r="K107" s="13"/>
-      <c r="L107" s="13"/>
-      <c r="M107" s="13"/>
-      <c r="N107" s="14"/>
-    </row>
-    <row r="108" spans="2:14" ht="15.75">
+      <c r="J107" s="15"/>
+      <c r="K107" s="15"/>
+      <c r="L107" s="15"/>
+      <c r="M107" s="15"/>
+      <c r="N107" s="16"/>
+    </row>
+    <row r="108" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B108" s="5" t="s">
         <v>310</v>
       </c>
@@ -5248,18 +5260,18 @@
         <v>375</v>
       </c>
       <c r="H108" s="1"/>
-      <c r="I108" s="15" t="s">
+      <c r="I108" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="J108" s="16" t="s">
+      <c r="J108" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="K108" s="16"/>
-      <c r="L108" s="16"/>
-      <c r="M108" s="16"/>
-      <c r="N108" s="17"/>
-    </row>
-    <row r="109" spans="2:14" ht="15" customHeight="1">
+      <c r="K108" s="12"/>
+      <c r="L108" s="12"/>
+      <c r="M108" s="12"/>
+      <c r="N108" s="13"/>
+    </row>
+    <row r="109" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B109" s="5" t="s">
         <v>346</v>
       </c>
@@ -5279,18 +5291,18 @@
         <v>375</v>
       </c>
       <c r="H109" s="1"/>
-      <c r="I109" s="15"/>
-      <c r="J109" s="16" t="s">
+      <c r="I109" s="17"/>
+      <c r="J109" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="K109" s="16"/>
-      <c r="L109" s="17"/>
-      <c r="M109" s="16" t="s">
+      <c r="K109" s="12"/>
+      <c r="L109" s="13"/>
+      <c r="M109" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N109" s="17"/>
-    </row>
-    <row r="110" spans="2:14" ht="15.75">
+      <c r="N109" s="13"/>
+    </row>
+    <row r="110" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B110" s="5" t="s">
         <v>356</v>
       </c>
@@ -5327,7 +5339,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="111" spans="2:14" ht="15">
+    <row r="111" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B111" s="5" t="s">
         <v>393</v>
       </c>
@@ -5366,7 +5378,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="112" spans="2:14" ht="15">
+    <row r="112" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B112" s="5" t="s">
         <v>40</v>
       </c>
@@ -5405,7 +5417,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="113" spans="2:14" ht="15">
+    <row r="113" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B113" s="5" t="s">
         <v>49</v>
       </c>
@@ -5444,7 +5456,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="114" spans="2:14" ht="15">
+    <row r="114" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
       <c r="D114" s="1"/>
@@ -5471,7 +5483,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="115" spans="2:14" ht="15">
+    <row r="115" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
       <c r="D115" s="1"/>
@@ -5486,72 +5498,72 @@
       <c r="M115" s="1"/>
       <c r="N115" s="1"/>
     </row>
-    <row r="116" spans="2:14" ht="15" customHeight="1">
-      <c r="B116" s="12" t="s">
+    <row r="116" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B116" s="14" t="s">
         <v>410</v>
       </c>
-      <c r="C116" s="13"/>
-      <c r="D116" s="13"/>
-      <c r="E116" s="13"/>
-      <c r="F116" s="13"/>
-      <c r="G116" s="14"/>
+      <c r="C116" s="15"/>
+      <c r="D116" s="15"/>
+      <c r="E116" s="15"/>
+      <c r="F116" s="15"/>
+      <c r="G116" s="16"/>
       <c r="H116" s="1"/>
-      <c r="I116" s="12" t="s">
+      <c r="I116" s="14" t="s">
         <v>411</v>
       </c>
-      <c r="J116" s="13"/>
-      <c r="K116" s="13"/>
-      <c r="L116" s="13"/>
-      <c r="M116" s="13"/>
-      <c r="N116" s="14"/>
-    </row>
-    <row r="117" spans="2:14" ht="15" customHeight="1">
-      <c r="B117" s="15" t="s">
+      <c r="J116" s="15"/>
+      <c r="K116" s="15"/>
+      <c r="L116" s="15"/>
+      <c r="M116" s="15"/>
+      <c r="N116" s="16"/>
+    </row>
+    <row r="117" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B117" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C117" s="16" t="s">
+      <c r="C117" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D117" s="16"/>
-      <c r="E117" s="16"/>
-      <c r="F117" s="16"/>
-      <c r="G117" s="17"/>
+      <c r="D117" s="12"/>
+      <c r="E117" s="12"/>
+      <c r="F117" s="12"/>
+      <c r="G117" s="13"/>
       <c r="H117" s="1"/>
-      <c r="I117" s="15" t="s">
+      <c r="I117" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="J117" s="16" t="s">
+      <c r="J117" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="K117" s="16"/>
-      <c r="L117" s="16"/>
-      <c r="M117" s="16"/>
-      <c r="N117" s="17"/>
-    </row>
-    <row r="118" spans="2:14" ht="15" customHeight="1">
-      <c r="B118" s="15"/>
-      <c r="C118" s="16" t="s">
+      <c r="K117" s="12"/>
+      <c r="L117" s="12"/>
+      <c r="M117" s="12"/>
+      <c r="N117" s="13"/>
+    </row>
+    <row r="118" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B118" s="17"/>
+      <c r="C118" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D118" s="16"/>
-      <c r="E118" s="17"/>
-      <c r="F118" s="16" t="s">
+      <c r="D118" s="12"/>
+      <c r="E118" s="13"/>
+      <c r="F118" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G118" s="17"/>
+      <c r="G118" s="13"/>
       <c r="H118" s="1"/>
-      <c r="I118" s="15"/>
-      <c r="J118" s="16" t="s">
+      <c r="I118" s="17"/>
+      <c r="J118" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="K118" s="16"/>
-      <c r="L118" s="17"/>
-      <c r="M118" s="16" t="s">
+      <c r="K118" s="12"/>
+      <c r="L118" s="13"/>
+      <c r="M118" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N118" s="17"/>
-    </row>
-    <row r="119" spans="2:14" ht="15.75">
+      <c r="N118" s="13"/>
+    </row>
+    <row r="119" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B119" s="18"/>
       <c r="C119" s="2" t="s">
         <v>412</v>
@@ -5586,7 +5598,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="120" spans="2:14" ht="15">
+    <row r="120" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B120" s="5" t="s">
         <v>345</v>
       </c>
@@ -5625,7 +5637,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="121" spans="2:14" ht="15">
+    <row r="121" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B121" s="5" t="s">
         <v>300</v>
       </c>
@@ -5664,7 +5676,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="122" spans="2:14" ht="15">
+    <row r="122" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B122" s="5" t="s">
         <v>305</v>
       </c>
@@ -5703,7 +5715,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="123" spans="2:14" ht="15">
+    <row r="123" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B123" s="5" t="s">
         <v>310</v>
       </c>
@@ -5742,7 +5754,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="124" spans="2:14" ht="15">
+    <row r="124" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B124" s="5" t="s">
         <v>40</v>
       </c>
@@ -5781,7 +5793,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="125" spans="2:14" ht="15">
+    <row r="125" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B125" s="5" t="s">
         <v>49</v>
       </c>
@@ -5820,7 +5832,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="126" spans="2:14" ht="15">
+    <row r="126" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
       <c r="D126" s="1"/>
@@ -5835,15 +5847,15 @@
       <c r="M126" s="1"/>
       <c r="N126" s="1"/>
     </row>
-    <row r="127" spans="2:14" ht="18.75">
-      <c r="B127" s="12" t="s">
+    <row r="127" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B127" s="14" t="s">
         <v>444</v>
       </c>
-      <c r="C127" s="13"/>
-      <c r="D127" s="13"/>
-      <c r="E127" s="13"/>
-      <c r="F127" s="13"/>
-      <c r="G127" s="14"/>
+      <c r="C127" s="15"/>
+      <c r="D127" s="15"/>
+      <c r="E127" s="15"/>
+      <c r="F127" s="15"/>
+      <c r="G127" s="16"/>
       <c r="H127" s="1"/>
       <c r="I127" s="1"/>
       <c r="J127" s="1"/>
@@ -5852,17 +5864,17 @@
       <c r="M127" s="1"/>
       <c r="N127" s="1"/>
     </row>
-    <row r="128" spans="2:14" ht="15.75">
-      <c r="B128" s="15" t="s">
+    <row r="128" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B128" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C128" s="16" t="s">
+      <c r="C128" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D128" s="16"/>
-      <c r="E128" s="16"/>
-      <c r="F128" s="16"/>
-      <c r="G128" s="17"/>
+      <c r="D128" s="12"/>
+      <c r="E128" s="12"/>
+      <c r="F128" s="12"/>
+      <c r="G128" s="13"/>
       <c r="H128" s="1"/>
       <c r="I128" s="1"/>
       <c r="J128" s="1"/>
@@ -5871,17 +5883,17 @@
       <c r="M128" s="1"/>
       <c r="N128" s="1"/>
     </row>
-    <row r="129" spans="2:14" ht="15" customHeight="1">
-      <c r="B129" s="15"/>
-      <c r="C129" s="16" t="s">
+    <row r="129" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B129" s="17"/>
+      <c r="C129" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D129" s="16"/>
-      <c r="E129" s="17"/>
-      <c r="F129" s="16" t="s">
+      <c r="D129" s="12"/>
+      <c r="E129" s="13"/>
+      <c r="F129" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G129" s="17"/>
+      <c r="G129" s="13"/>
       <c r="H129" s="1"/>
       <c r="I129" s="1"/>
       <c r="J129" s="1"/>
@@ -5890,7 +5902,7 @@
       <c r="M129" s="1"/>
       <c r="N129" s="1"/>
     </row>
-    <row r="130" spans="2:14" ht="15.75">
+    <row r="130" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B130" s="18"/>
       <c r="C130" s="2" t="s">
         <v>445</v>
@@ -5915,7 +5927,7 @@
       <c r="M130" s="1"/>
       <c r="N130" s="1"/>
     </row>
-    <row r="131" spans="2:14" ht="15">
+    <row r="131" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B131" s="10" t="s">
         <v>300</v>
       </c>
@@ -5942,7 +5954,7 @@
       <c r="M131" s="1"/>
       <c r="N131" s="1"/>
     </row>
-    <row r="132" spans="2:14" ht="15">
+    <row r="132" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B132" s="5" t="s">
         <v>305</v>
       </c>
@@ -5969,7 +5981,7 @@
       <c r="M132" s="1"/>
       <c r="N132" s="1"/>
     </row>
-    <row r="133" spans="2:14" ht="15">
+    <row r="133" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B133" s="5" t="s">
         <v>310</v>
       </c>
@@ -5996,7 +6008,7 @@
       <c r="M133" s="1"/>
       <c r="N133" s="1"/>
     </row>
-    <row r="134" spans="2:14" ht="15">
+    <row r="134" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B134" s="5" t="s">
         <v>356</v>
       </c>
@@ -6023,7 +6035,7 @@
       <c r="M134" s="1"/>
       <c r="N134" s="1"/>
     </row>
-    <row r="135" spans="2:14" ht="15">
+    <row r="135" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B135" s="5" t="s">
         <v>393</v>
       </c>
@@ -6050,7 +6062,7 @@
       <c r="M135" s="1"/>
       <c r="N135" s="1"/>
     </row>
-    <row r="136" spans="2:14" ht="15">
+    <row r="136" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B136" s="5" t="s">
         <v>40</v>
       </c>
@@ -6077,7 +6089,7 @@
       <c r="M136" s="1"/>
       <c r="N136" s="1"/>
     </row>
-    <row r="137" spans="2:14" ht="15">
+    <row r="137" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B137" s="5" t="s">
         <v>49</v>
       </c>
@@ -6104,10 +6116,104 @@
       <c r="M137" s="1"/>
       <c r="N137" s="1"/>
     </row>
-    <row r="138" spans="2:14" ht="15"/>
-    <row r="139" spans="2:14" ht="15"/>
   </sheetData>
   <mergeCells count="120">
+    <mergeCell ref="B127:G127"/>
+    <mergeCell ref="B128:B130"/>
+    <mergeCell ref="C128:G128"/>
+    <mergeCell ref="C129:E129"/>
+    <mergeCell ref="F129:G129"/>
+    <mergeCell ref="B116:G116"/>
+    <mergeCell ref="I116:N116"/>
+    <mergeCell ref="B117:B119"/>
+    <mergeCell ref="C117:G117"/>
+    <mergeCell ref="I117:I119"/>
+    <mergeCell ref="J117:N117"/>
+    <mergeCell ref="C118:E118"/>
+    <mergeCell ref="F118:G118"/>
+    <mergeCell ref="J118:L118"/>
+    <mergeCell ref="M118:N118"/>
+    <mergeCell ref="I107:N107"/>
+    <mergeCell ref="I108:I110"/>
+    <mergeCell ref="J108:N108"/>
+    <mergeCell ref="J109:L109"/>
+    <mergeCell ref="M109:N109"/>
+    <mergeCell ref="B98:G98"/>
+    <mergeCell ref="I98:N98"/>
+    <mergeCell ref="B99:B101"/>
+    <mergeCell ref="C99:G99"/>
+    <mergeCell ref="I99:I101"/>
+    <mergeCell ref="J99:N99"/>
+    <mergeCell ref="C100:E100"/>
+    <mergeCell ref="F100:G100"/>
+    <mergeCell ref="J100:L100"/>
+    <mergeCell ref="M100:N100"/>
+    <mergeCell ref="B83:G83"/>
+    <mergeCell ref="I83:N83"/>
+    <mergeCell ref="B84:B86"/>
+    <mergeCell ref="C84:G84"/>
+    <mergeCell ref="I84:I86"/>
+    <mergeCell ref="J84:N84"/>
+    <mergeCell ref="C85:E85"/>
+    <mergeCell ref="F85:G85"/>
+    <mergeCell ref="J85:L85"/>
+    <mergeCell ref="M85:N85"/>
+    <mergeCell ref="I44:N44"/>
+    <mergeCell ref="I45:I47"/>
+    <mergeCell ref="J45:N45"/>
+    <mergeCell ref="B64:G64"/>
+    <mergeCell ref="B65:B67"/>
+    <mergeCell ref="C65:G65"/>
+    <mergeCell ref="B73:G73"/>
+    <mergeCell ref="I73:N73"/>
+    <mergeCell ref="B74:B76"/>
+    <mergeCell ref="C74:G74"/>
+    <mergeCell ref="I74:I76"/>
+    <mergeCell ref="J74:N74"/>
+    <mergeCell ref="C75:E75"/>
+    <mergeCell ref="F75:G75"/>
+    <mergeCell ref="J75:L75"/>
+    <mergeCell ref="M75:N75"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:G38"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="J2:N2"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="I11:N11"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="J12:N12"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="I29:I31"/>
+    <mergeCell ref="J29:N29"/>
+    <mergeCell ref="J30:L30"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="I20:I22"/>
+    <mergeCell ref="J20:N20"/>
+    <mergeCell ref="J21:L21"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="I28:N28"/>
+    <mergeCell ref="I19:N19"/>
     <mergeCell ref="C66:E66"/>
     <mergeCell ref="F66:G66"/>
     <mergeCell ref="J46:L46"/>
@@ -6129,105 +6235,9 @@
     <mergeCell ref="M56:N56"/>
     <mergeCell ref="I64:N64"/>
     <mergeCell ref="I65:I67"/>
-    <mergeCell ref="I11:N11"/>
-    <mergeCell ref="I12:I14"/>
-    <mergeCell ref="J12:N12"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="I29:I31"/>
-    <mergeCell ref="J29:N29"/>
-    <mergeCell ref="J30:L30"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="I20:I22"/>
-    <mergeCell ref="J20:N20"/>
-    <mergeCell ref="J21:L21"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="I28:N28"/>
-    <mergeCell ref="I19:N19"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="I1:N1"/>
-    <mergeCell ref="I2:I4"/>
-    <mergeCell ref="J2:N2"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="M3:N3"/>
     <mergeCell ref="J65:N65"/>
     <mergeCell ref="J66:L66"/>
     <mergeCell ref="M66:N66"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:G38"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="I44:N44"/>
-    <mergeCell ref="I45:I47"/>
-    <mergeCell ref="J45:N45"/>
-    <mergeCell ref="B64:G64"/>
-    <mergeCell ref="B65:B67"/>
-    <mergeCell ref="C65:G65"/>
-    <mergeCell ref="B73:G73"/>
-    <mergeCell ref="I73:N73"/>
-    <mergeCell ref="B74:B76"/>
-    <mergeCell ref="C74:G74"/>
-    <mergeCell ref="I74:I76"/>
-    <mergeCell ref="J74:N74"/>
-    <mergeCell ref="C75:E75"/>
-    <mergeCell ref="F75:G75"/>
-    <mergeCell ref="J75:L75"/>
-    <mergeCell ref="M75:N75"/>
-    <mergeCell ref="B83:G83"/>
-    <mergeCell ref="I83:N83"/>
-    <mergeCell ref="B84:B86"/>
-    <mergeCell ref="C84:G84"/>
-    <mergeCell ref="I84:I86"/>
-    <mergeCell ref="J84:N84"/>
-    <mergeCell ref="C85:E85"/>
-    <mergeCell ref="F85:G85"/>
-    <mergeCell ref="J85:L85"/>
-    <mergeCell ref="M85:N85"/>
-    <mergeCell ref="I107:N107"/>
-    <mergeCell ref="I108:I110"/>
-    <mergeCell ref="J108:N108"/>
-    <mergeCell ref="J109:L109"/>
-    <mergeCell ref="M109:N109"/>
-    <mergeCell ref="B98:G98"/>
-    <mergeCell ref="I98:N98"/>
-    <mergeCell ref="B99:B101"/>
-    <mergeCell ref="C99:G99"/>
-    <mergeCell ref="I99:I101"/>
-    <mergeCell ref="J99:N99"/>
-    <mergeCell ref="C100:E100"/>
-    <mergeCell ref="F100:G100"/>
-    <mergeCell ref="J100:L100"/>
-    <mergeCell ref="M100:N100"/>
-    <mergeCell ref="B127:G127"/>
-    <mergeCell ref="B128:B130"/>
-    <mergeCell ref="C128:G128"/>
-    <mergeCell ref="C129:E129"/>
-    <mergeCell ref="F129:G129"/>
-    <mergeCell ref="B116:G116"/>
-    <mergeCell ref="I116:N116"/>
-    <mergeCell ref="B117:B119"/>
-    <mergeCell ref="C117:G117"/>
-    <mergeCell ref="I117:I119"/>
-    <mergeCell ref="J117:N117"/>
-    <mergeCell ref="C118:E118"/>
-    <mergeCell ref="F118:G118"/>
-    <mergeCell ref="J118:L118"/>
-    <mergeCell ref="M118:N118"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -6235,14 +6245,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="2d881088-f327-4930-bfe4-ce7a6da610bd" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7d49c0e8-093d-4e35-ba10-2ef43e532370">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6441,22 +6449,50 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="2d881088-f327-4930-bfe4-ce7a6da610bd" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7d49c0e8-093d-4e35-ba10-2ef43e532370">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70DF1220-3262-4773-A79F-083079DCC3A2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5765D775-FF1F-47E5-AC14-0AFAE867B5EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CF5FE5C-B69E-4F1A-AA1D-6FAD11F77B0A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CF5FE5C-B69E-4F1A-AA1D-6FAD11F77B0A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="7d49c0e8-093d-4e35-ba10-2ef43e532370"/>
+    <ds:schemaRef ds:uri="2d881088-f327-4930-bfe4-ce7a6da610bd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5765D775-FF1F-47E5-AC14-0AFAE867B5EA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70DF1220-3262-4773-A79F-083079DCC3A2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2d881088-f327-4930-bfe4-ce7a6da610bd"/>
+    <ds:schemaRef ds:uri="7d49c0e8-093d-4e35-ba10-2ef43e532370"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>